<commit_message>
Signed-off-by: STUDENT Darragh M. Sweeney <Darragh.M.Sweeney@students.ittralee.ie>
</commit_message>
<xml_diff>
--- a/D_Framework.xlsx
+++ b/D_Framework.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darra\Desktop\CG\ExcelPowepoint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00211528\Desktop\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0ACA6EE-FD8C-4956-8D9D-A05667571F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1640BCFB-4F2F-457F-A9A5-6D0F32506C3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{4CCA19A7-95F2-4BD1-A2B8-EC6EDDEFA500}"/>
   </bookViews>
@@ -114,9 +114,6 @@
     <t>(22,21,20)</t>
   </si>
   <si>
-    <t>(21,15,20)</t>
-  </si>
-  <si>
     <t>(19,15,20)</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
   </si>
   <si>
     <t>(0,16,2)</t>
-  </si>
-  <si>
-    <t>(2,16,3)</t>
   </si>
   <si>
     <t>(2,17,3)</t>
@@ -145,12 +139,6 @@
   </si>
   <si>
     <t>(5,21,7)</t>
-  </si>
-  <si>
-    <t>(21,7,8)</t>
-  </si>
-  <si>
-    <t>(21,8,22)</t>
   </si>
   <si>
     <t>(22,24,10)</t>
@@ -180,12 +168,6 @@
     <t>(11,27,25)</t>
   </si>
   <si>
-    <t>(4,18,23)</t>
-  </si>
-  <si>
-    <t>(4,23,9)</t>
-  </si>
-  <si>
     <t>Top</t>
   </si>
   <si>
@@ -198,22 +180,40 @@
     <t>(0,15,14)</t>
   </si>
   <si>
-    <t>(23,24,10)</t>
-  </si>
-  <si>
-    <t>(23,10,9)</t>
-  </si>
-  <si>
     <t>(26,27,13)</t>
   </si>
   <si>
-    <t>(26,13,14)</t>
+    <t>(21,19,20)</t>
   </si>
   <si>
-    <t>(4,5,19)</t>
+    <t>(2,16,17)</t>
   </si>
   <si>
-    <t>(4,19,18)</t>
+    <t>(26,13,12)</t>
+  </si>
+  <si>
+    <t>(5,4,19)</t>
+  </si>
+  <si>
+    <t>(4,18,19)</t>
+  </si>
+  <si>
+    <t>(24,23,10)</t>
+  </si>
+  <si>
+    <t>(10,23,9)</t>
+  </si>
+  <si>
+    <t>(7,21,8)</t>
+  </si>
+  <si>
+    <t>(8,21,22)</t>
+  </si>
+  <si>
+    <t>(18,4,23)</t>
+  </si>
+  <si>
+    <t>(23,4,9)</t>
   </si>
 </sst>
 </file>
@@ -5651,8 +5651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2D2B34-4B2E-4F96-A95E-A8C94726318D}">
   <dimension ref="B7:T195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5896,7 +5896,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
@@ -5904,7 +5904,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
@@ -5912,7 +5912,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
@@ -5920,7 +5920,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
@@ -5928,7 +5928,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
@@ -5936,7 +5936,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
@@ -5944,7 +5944,7 @@
         <v>7</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
@@ -5952,7 +5952,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
@@ -5960,15 +5960,15 @@
         <v>9</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>40</v>
+      <c r="C33" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -5976,7 +5976,7 @@
         <v>11</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -5984,7 +5984,7 @@
         <v>12</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -5992,7 +5992,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
@@ -6012,7 +6012,7 @@
         <v>16</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
@@ -6020,7 +6020,7 @@
         <v>17</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
@@ -6028,7 +6028,7 @@
         <v>18</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
@@ -6036,7 +6036,7 @@
         <v>19</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
@@ -6044,7 +6044,7 @@
         <v>20</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
@@ -6052,7 +6052,7 @@
         <v>21</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
@@ -6060,15 +6060,15 @@
         <v>22</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>51</v>
+      <c r="C46" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
@@ -6076,20 +6076,18 @@
         <v>24</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="5"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="5"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
@@ -6105,38 +6103,38 @@
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="5"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="5"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="C53" s="3"/>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
@@ -6144,7 +6142,7 @@
         <v>57</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
@@ -6152,7 +6150,7 @@
         <v>58</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>